<commit_message>
Fix equation for inversion of delta and get new results
</commit_message>
<xml_diff>
--- a/results/xgbr_wSOFA.xlsx
+++ b/results/xgbr_wSOFA.xlsx
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.274</v>
+        <v>0.218</v>
       </c>
       <c r="C7" t="n">
-        <v>0.648</v>
+        <v>0.676</v>
       </c>
       <c r="D7" t="n">
-        <v>0.44</v>
+        <v>0.468</v>
       </c>
       <c r="E7" t="n">
-        <v>0.615</v>
+        <v>0.628</v>
       </c>
       <c r="F7" t="n">
-        <v>0.434</v>
+        <v>0.462</v>
       </c>
       <c r="G7" t="n">
-        <v>0.492</v>
+        <v>0.515</v>
       </c>
     </row>
     <row r="8">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-14.819</v>
+        <v>-16.055</v>
       </c>
       <c r="C8" t="n">
-        <v>0.406</v>
+        <v>0.453</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.802</v>
+        <v>-1.659</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.574</v>
       </c>
       <c r="F8" t="n">
-        <v>0.412</v>
+        <v>0.441</v>
       </c>
       <c r="G8" t="n">
-        <v>0.479</v>
+        <v>0.502</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.536</v>
+        <v>2.633</v>
       </c>
       <c r="C9" t="n">
-        <v>2.097</v>
+        <v>2.012</v>
       </c>
       <c r="D9" t="n">
-        <v>2.353</v>
+        <v>2.292</v>
       </c>
       <c r="E9" t="n">
-        <v>2.35</v>
+        <v>2.31</v>
       </c>
       <c r="F9" t="n">
-        <v>2.489</v>
+        <v>2.426</v>
       </c>
       <c r="G9" t="n">
-        <v>2.436</v>
+        <v>2.381</v>
       </c>
     </row>
     <row r="10">
@@ -675,19 +675,19 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
         <v>44</v>
       </c>
       <c r="G10" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9429999999999999</v>
+        <v>0.886</v>
       </c>
       <c r="C11" t="n">
-        <v>0.335</v>
+        <v>0.363</v>
       </c>
       <c r="D11" t="n">
-        <v>0.497</v>
+        <v>0.525</v>
       </c>
       <c r="E11" t="n">
-        <v>0.617</v>
+        <v>0.63</v>
       </c>
       <c r="F11" t="n">
-        <v>0.466</v>
+        <v>0.495</v>
       </c>
       <c r="G11" t="n">
-        <v>0.503</v>
+        <v>0.526</v>
       </c>
     </row>
     <row r="12">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>20.561</v>
+        <v>19.325</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.613</v>
       </c>
       <c r="D12" t="n">
-        <v>2.483</v>
+        <v>2.626</v>
       </c>
       <c r="E12" t="n">
-        <v>0.707</v>
+        <v>0.722</v>
       </c>
       <c r="F12" t="n">
-        <v>0.484</v>
+        <v>0.514</v>
       </c>
       <c r="G12" t="n">
-        <v>0.516</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="13">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.31</v>
+        <v>-1.213</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.834</v>
+        <v>-0.918</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.878</v>
+        <v>-0.9389999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.44</v>
+        <v>-1.48</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.872</v>
+        <v>-0.9360000000000001</v>
       </c>
       <c r="G13" t="n">
-        <v>-1</v>
+        <v>-1.056</v>
       </c>
     </row>
     <row r="14">
@@ -775,19 +775,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
         <v>0</v>
       </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
       <c r="E14" t="n">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="F14" t="n">
         <v>-3</v>
       </c>
       <c r="G14" t="n">
-        <v>-10</v>
+        <v>-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>